<commit_message>
proc enum in struct
</commit_message>
<xml_diff>
--- a/data_xlsx/data_excel.xlsx
+++ b/data_xlsx/data_excel.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +432,7 @@
     <col width="80" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,6 +469,11 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>Contain_size</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Primitive_ID</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1129,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
@@ -1175,7 +1181,7 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
@@ -1227,7 +1233,7 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
@@ -1279,7 +1285,7 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
@@ -1331,7 +1337,7 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
@@ -1383,7 +1389,7 @@
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
@@ -1434,7 +1440,9 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="n">
+        <v>-1</v>
+      </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
@@ -1481,7 +1489,7 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
@@ -1529,7 +1537,7 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
@@ -1576,7 +1584,9 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="n">
+        <v>-1</v>
+      </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
@@ -1622,7 +1632,9 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="n">
+        <v>-1</v>
+      </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
@@ -1672,7 +1684,9 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
+      <c r="N13" t="n">
+        <v>-1</v>
+      </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
@@ -1722,7 +1736,9 @@
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+      <c r="N14" t="n">
+        <v>-1</v>
+      </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
@@ -1772,7 +1788,9 @@
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+      <c r="N15" t="n">
+        <v>-1</v>
+      </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
@@ -1822,7 +1840,9 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+      <c r="N16" t="n">
+        <v>-1</v>
+      </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
@@ -1872,7 +1892,9 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
+      <c r="N17" t="n">
+        <v>-1</v>
+      </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
@@ -1922,7 +1944,9 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+      <c r="N18" t="n">
+        <v>-1</v>
+      </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
@@ -1972,7 +1996,9 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+      <c r="N19" t="n">
+        <v>-1</v>
+      </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
@@ -2022,7 +2048,9 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+      <c r="N20" t="n">
+        <v>-1</v>
+      </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
@@ -2072,7 +2100,9 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
+      <c r="N21" t="n">
+        <v>-1</v>
+      </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
@@ -2122,7 +2152,9 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+      <c r="N22" t="n">
+        <v>-1</v>
+      </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
@@ -2172,7 +2204,9 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+      <c r="N23" t="n">
+        <v>-1</v>
+      </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
@@ -2219,7 +2253,7 @@
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
@@ -2267,7 +2301,7 @@
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
@@ -2315,7 +2349,7 @@
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
@@ -2362,7 +2396,9 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
+      <c r="N27" t="n">
+        <v>-1</v>
+      </c>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
@@ -2409,7 +2445,7 @@
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
@@ -2460,7 +2496,9 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
+      <c r="N29" t="n">
+        <v>-1</v>
+      </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
@@ -2510,7 +2548,9 @@
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
+      <c r="N30" t="n">
+        <v>-1</v>
+      </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
@@ -2556,7 +2596,9 @@
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
+      <c r="N31" t="n">
+        <v>-1</v>
+      </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
@@ -2602,7 +2644,9 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
+      <c r="N32" t="n">
+        <v>-1</v>
+      </c>
       <c r="O32" t="inlineStr">
         <is>
           <t>E2setupResponse</t>
@@ -2677,7 +2721,7 @@
         </is>
       </c>
       <c r="N33" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr"/>
@@ -2736,7 +2780,9 @@
           <t>child_of_msg</t>
         </is>
       </c>
-      <c r="N34" t="inlineStr"/>
+      <c r="N34" t="n">
+        <v>-1</v>
+      </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
@@ -2798,7 +2844,9 @@
           <t>child_of_msg</t>
         </is>
       </c>
-      <c r="N35" t="inlineStr"/>
+      <c r="N35" t="n">
+        <v>-1</v>
+      </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
@@ -2860,7 +2908,9 @@
           <t>child_of_msg</t>
         </is>
       </c>
-      <c r="N36" t="inlineStr"/>
+      <c r="N36" t="n">
+        <v>-1</v>
+      </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
@@ -2918,7 +2968,9 @@
           <t>child_of_msg</t>
         </is>
       </c>
-      <c r="N37" t="inlineStr"/>
+      <c r="N37" t="n">
+        <v>-1</v>
+      </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
@@ -2972,7 +3024,9 @@
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
+      <c r="N38" t="n">
+        <v>-1</v>
+      </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
@@ -3022,7 +3076,9 @@
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
+      <c r="N39" t="n">
+        <v>-1</v>
+      </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
@@ -3072,7 +3128,9 @@
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
+      <c r="N40" t="n">
+        <v>-1</v>
+      </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
@@ -3122,7 +3180,9 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
+      <c r="N41" t="n">
+        <v>-1</v>
+      </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
@@ -3172,7 +3232,9 @@
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
+      <c r="N42" t="n">
+        <v>-1</v>
+      </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
@@ -3222,7 +3284,9 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
+      <c r="N43" t="n">
+        <v>-1</v>
+      </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
@@ -3272,7 +3336,9 @@
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
+      <c r="N44" t="n">
+        <v>-1</v>
+      </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
@@ -3322,7 +3388,9 @@
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
+      <c r="N45" t="n">
+        <v>-1</v>
+      </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
@@ -3372,7 +3440,9 @@
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
+      <c r="N46" t="n">
+        <v>-1</v>
+      </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
@@ -3419,7 +3489,7 @@
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr"/>
@@ -3466,7 +3536,9 @@
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
+      <c r="N48" t="n">
+        <v>-1</v>
+      </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
@@ -3516,7 +3588,9 @@
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
+      <c r="N49" t="n">
+        <v>-1</v>
+      </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
@@ -3566,7 +3640,9 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
+      <c r="N50" t="n">
+        <v>-1</v>
+      </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
@@ -3613,7 +3689,7 @@
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
@@ -3660,7 +3736,9 @@
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
+      <c r="N52" t="n">
+        <v>-1</v>
+      </c>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
@@ -3707,7 +3785,7 @@
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
@@ -3754,7 +3832,9 @@
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
+      <c r="N54" t="n">
+        <v>-1</v>
+      </c>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
@@ -3801,7 +3881,7 @@
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
@@ -3848,7 +3928,9 @@
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
       <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
+      <c r="N56" t="n">
+        <v>-1</v>
+      </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
@@ -3895,7 +3977,7 @@
       <c r="L57" t="inlineStr"/>
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
@@ -3942,7 +4024,9 @@
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
       <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
+      <c r="N58" t="n">
+        <v>-1</v>
+      </c>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
@@ -3989,7 +4073,7 @@
       <c r="L59" t="inlineStr"/>
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
@@ -4037,7 +4121,7 @@
       <c r="L60" t="inlineStr"/>
       <c r="M60" t="inlineStr"/>
       <c r="N60" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
@@ -4088,7 +4172,9 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
       <c r="M61" t="inlineStr"/>
-      <c r="N61" t="inlineStr"/>
+      <c r="N61" t="n">
+        <v>-1</v>
+      </c>
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
@@ -4135,7 +4221,7 @@
       <c r="L62" t="inlineStr"/>
       <c r="M62" t="inlineStr"/>
       <c r="N62" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr"/>
@@ -4182,7 +4268,9 @@
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
       <c r="M63" t="inlineStr"/>
-      <c r="N63" t="inlineStr"/>
+      <c r="N63" t="n">
+        <v>-1</v>
+      </c>
       <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr"/>
       <c r="Q63" t="inlineStr"/>
@@ -4232,7 +4320,9 @@
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr"/>
       <c r="M64" t="inlineStr"/>
-      <c r="N64" t="inlineStr"/>
+      <c r="N64" t="n">
+        <v>-1</v>
+      </c>
       <c r="O64" t="inlineStr"/>
       <c r="P64" t="inlineStr"/>
       <c r="Q64" t="inlineStr"/>
@@ -4282,7 +4372,9 @@
       </c>
       <c r="L65" t="inlineStr"/>
       <c r="M65" t="inlineStr"/>
-      <c r="N65" t="inlineStr"/>
+      <c r="N65" t="n">
+        <v>-1</v>
+      </c>
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
@@ -4332,7 +4424,9 @@
       </c>
       <c r="L66" t="inlineStr"/>
       <c r="M66" t="inlineStr"/>
-      <c r="N66" t="inlineStr"/>
+      <c r="N66" t="n">
+        <v>-1</v>
+      </c>
       <c r="O66" t="inlineStr"/>
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="inlineStr"/>

</xml_diff>

<commit_message>
process primtive and fix chocie
</commit_message>
<xml_diff>
--- a/data_xlsx/data_excel.xlsx
+++ b/data_xlsx/data_excel.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,10 +425,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="19" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
     <col width="5" customWidth="1" min="3" max="3"/>
-    <col width="6" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="80" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
@@ -480,19 +480,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CauseE2node</t>
+          <t>AMFName</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"e2node-component-unknown","e2node-component-unknown")]</t>
-        </is>
-      </c>
+          <t>PrintableString (SIZE(1..150, ...))</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>1</t>
@@ -507,7 +513,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CauseMisc</t>
+          <t>CauseE2node</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -517,7 +523,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>[(0,"control-processing-overload","control-processing-overload"),(1,"hardware-failure","hardware-failure"),(2,"om-intervention","om-intervention"),(3,"unspecified","unspecified")]</t>
+          <t>[(0,"e2node-component-unknown","e2node-component-unknown")]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -534,7 +540,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CauseProtocol</t>
+          <t>CauseMisc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -544,7 +550,7 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>[(0,"transfer-syntax-error","transfer-syntax-error"),(1,"abstract-syntax-error-reject","abstract-syntax-error-reject"),(2,"abstract-syntax-error-ignore-and-notify","abstract-syntax-error-ignore-and-notify"),(3,"message-not-compatible-with-receiver-state","message-not-compatible-with-receiver-state"),(4,"semantic-error","semantic-error"),(5,"abstract-syntax-error-falsely-constructed-message","abstract-syntax-error-falsely-constructed-message"),(6,"unspecified","unspecified")]</t>
+          <t>[(0,"control-processing-overload","control-processing-overload"),(1,"hardware-failure","hardware-failure"),(2,"om-intervention","om-intervention"),(3,"unspecified","unspecified")]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -561,7 +567,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CauseRICrequest</t>
+          <t>CauseProtocol</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -571,7 +577,7 @@
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>[(0,"ran-function-id-invalid","ran-function-id-invalid"),(1,"action-not-supported","action-not-supported"),(2,"excessive-actions","excessive-actions"),(3,"duplicate-action","duplicate-action"),(4,"duplicate-event-trigger","duplicate-event-trigger"),(5,"function-resource-limit","function-resource-limit"),(6,"request-id-unknown","request-id-unknown"),(7,"inconsistent-action-subsequent-action-sequence","inconsistent-action-subsequent-action-sequence"),(8,"control-message-invalid","control-message-invalid"),(9,"ric-call-process-id-invalid","ric-call-process-id-invalid"),(10,"control-timer-expired","control-timer-expired"),(11,"control-failed-to-execute","control-failed-to-execute"),(12,"system-not-ready","system-not-ready"),(13,"unspecified","unspecified"),(14,"ric-subscription-end-time-expired","ric-subscription-end-time-expired"),(15,"ric-subscription-end-time-invalid","ric-subscription-end-time-invalid"),(16,"duplicate-ric-request-id","duplicate-ric-request-id"),(17,"eventTriggerNotSupported","eventTriggerNotSupported"),(18,"requested-information-unavailable","requested-information-unavailable"),(19,"invalid-information-request","invalid-information-request")]</t>
+          <t>[(0,"transfer-syntax-error","transfer-syntax-error"),(1,"abstract-syntax-error-reject","abstract-syntax-error-reject"),(2,"abstract-syntax-error-ignore-and-notify","abstract-syntax-error-ignore-and-notify"),(3,"message-not-compatible-with-receiver-state","message-not-compatible-with-receiver-state"),(4,"semantic-error","semantic-error"),(5,"abstract-syntax-error-falsely-constructed-message","abstract-syntax-error-falsely-constructed-message"),(6,"unspecified","unspecified")]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -588,7 +594,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CauseRICservice</t>
+          <t>CauseRICrequest</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -598,7 +604,7 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>[(0,"ran-function-not-supported","ran-function-not-supported"),(1,"excessive-functions","excessive-functions"),(2,"ric-resource-limit","ric-resource-limit")]</t>
+          <t>[(0,"ran-function-id-invalid","ran-function-id-invalid"),(1,"action-not-supported","action-not-supported"),(2,"excessive-actions","excessive-actions"),(3,"duplicate-action","duplicate-action"),(4,"duplicate-event-trigger","duplicate-event-trigger"),(5,"function-resource-limit","function-resource-limit"),(6,"request-id-unknown","request-id-unknown"),(7,"inconsistent-action-subsequent-action-sequence","inconsistent-action-subsequent-action-sequence"),(8,"control-message-invalid","control-message-invalid"),(9,"ric-call-process-id-invalid","ric-call-process-id-invalid"),(10,"control-timer-expired","control-timer-expired"),(11,"control-failed-to-execute","control-failed-to-execute"),(12,"system-not-ready","system-not-ready"),(13,"unspecified","unspecified"),(14,"ric-subscription-end-time-expired","ric-subscription-end-time-expired"),(15,"ric-subscription-end-time-invalid","ric-subscription-end-time-invalid"),(16,"duplicate-ric-request-id","duplicate-ric-request-id"),(17,"eventTriggerNotSupported","eventTriggerNotSupported"),(18,"requested-information-unavailable","requested-information-unavailable"),(19,"invalid-information-request","invalid-information-request")]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -615,7 +621,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CauseTransport</t>
+          <t>CauseRICservice</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -625,7 +631,7 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>[(0,"unspecified","unspecified"),(1,"transport-resource-unavailable","transport-resource-unavailable")]</t>
+          <t>[(0,"ran-function-not-supported","ran-function-not-supported"),(1,"excessive-functions","excessive-functions"),(2,"ric-resource-limit","ric-resource-limit")]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -642,7 +648,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Criticality</t>
+          <t>CauseTransport</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -652,12 +658,12 @@
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>[(0,"reject","reject"),(1,"ignore","ignore"),(2,"notify","notify")]</t>
+          <t>[(0,"unspecified","unspecified"),(1,"transport-resource-unavailable","transport-resource-unavailable")]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -669,28 +675,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ProcedureCode</t>
+          <t>E2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>INTEGER (0..255)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>255</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr"/>
+          <t>ENUMERATED</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>[(0,"ng","ng"),(1,"xn","xn"),(2,"e1","e1"),(3,"f1","f1"),(4,"w1","w1"),(5,"s1","s1"),(6,"x2","x2")]</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -702,12 +702,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RANfunctionID</t>
+          <t>GNB-CU-UP-ID</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>INTEGER (0..4095)</t>
+          <t>INTEGER (0..68719476735)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4095</t>
+          <t>68719476735</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr"/>
@@ -735,12 +735,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ServiceLayerCause</t>
+          <t>GNB-DU-ID</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>OCTET STRING</t>
+          <t>INTEGER (0..68719476735)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>68719476735</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr"/>
@@ -758,25 +768,209 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>TriggeringMessage</t>
+          <t>MMEname</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ENUMERATED</t>
-        </is>
-      </c>
-      <c r="E12" s="1" t="inlineStr">
-        <is>
-          <t>[(0,"initiating-message","initiating-message"),(1,"successful-outcome","successful-outcome"),(2,"unsuccessfull-outcome","unsuccessfull-outcome")]</t>
-        </is>
-      </c>
+          <t>PrintableString (SIZE(1..150, ...))</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>NGENB-DU-ID</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>INTEGER (0..68719476735)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>68719476735</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>OCTET STRING (SIZE(3))</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>RANfunctionID</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>INTEGER (0..4095)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>4095</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>RANfunctionRevision</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>INTEGER (0..4095)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>4095</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ServiceLayerCause</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>OCTET STRING</t>
+        </is>
+      </c>
+      <c r="E17" s="1" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TransactionID</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>INTEGER (0..255,...)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>255</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>NULL</t>
         </is>
@@ -793,7 +987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -801,22 +995,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="32" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="32" customWidth="1" min="3" max="3"/>
+    <col width="42" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="42" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="32" customWidth="1" min="6" max="6"/>
+    <col width="42" customWidth="1" min="5" max="5"/>
+    <col width="42" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="11" customWidth="1" min="10" max="10"/>
-    <col width="11" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
+    <col width="23" customWidth="1" min="11" max="11"/>
+    <col width="56" customWidth="1" min="12" max="12"/>
     <col width="14" customWidth="1" min="13" max="13"/>
     <col width="7" customWidth="1" min="14" max="14"/>
     <col width="17" customWidth="1" min="15" max="15"/>
-    <col width="21" customWidth="1" min="16" max="16"/>
+    <col width="19" customWidth="1" min="16" max="16"/>
     <col width="14" customWidth="1" min="17" max="17"/>
     <col width="20" customWidth="1" min="18" max="18"/>
     <col width="16" customWidth="1" min="19" max="19"/>
@@ -1340,7 +1534,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1350,26 +1544,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>procedureCode</t>
+          <t>e2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="F10" s="1" t="inlineStr">
         <is>
-          <t>ProcedureCode</t>
+          <t>E2nodeComponentInterfaceType</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
           <t>1</t>
@@ -1380,7 +1570,7 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
@@ -1392,7 +1582,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1402,26 +1592,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>triggeringMessage</t>
+          <t>e2nodeComponentID</t>
         </is>
       </c>
       <c r="F11" s="1" t="inlineStr">
         <is>
-          <t>TriggeringMessage</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
           <t>1</t>
@@ -1432,7 +1618,7 @@
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
-        <v>13</v>
+        <v>-1</v>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
@@ -1444,7 +1630,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1454,26 +1640,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>procedureCriticality</t>
+          <t>e2nodeComponentConfigurationAck</t>
         </is>
       </c>
       <c r="F12" s="1" t="inlineStr">
         <is>
-          <t>Criticality</t>
+          <t>E2nodeComponentConfigurationAck</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>1</t>
@@ -1484,7 +1666,7 @@
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
-        <v>13</v>
+        <v>-1</v>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
@@ -1496,36 +1678,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-ItemIEs</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-ItemIEs</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>ricRequestorID</t>
+          <t>id-E2nodeComponentConfigAdditionAck-Item</t>
         </is>
       </c>
       <c r="F13" s="1" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+          <t>E2nodeComponentConfigAdditionAck-Item</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
           <t>1</t>
@@ -1548,43 +1730,43 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-List</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>CriticalityDiagnostics</t>
-        </is>
-      </c>
+          <t>SingleContainer</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>iEsCriticalityDiagnostics</t>
+          <t>E2nodeComponentConfigAdditionAck-List</t>
         </is>
       </c>
       <c r="F14" s="1" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentConfigAdditionAck-ItemIEs</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
@@ -1600,7 +1782,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentConfigurationAck</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1610,18 +1792,18 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentConfigurationAck</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>iECriticality</t>
+          <t>updateOutcome</t>
         </is>
       </c>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>Criticality</t>
+          <t>ENUMERATED</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -1633,10 +1815,14 @@
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>[(0, 'success', 'success'), (1, 'failure', 'failure')]</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>13</v>
+        <v>-1</v>
       </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
@@ -1648,7 +1834,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentConfigurationAck</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1658,22 +1844,26 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentConfigurationAck</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>iE-ID</t>
+          <t>failureCause</t>
         </is>
       </c>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>ProtocolIE-ID</t>
+          <t>Cause</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr">
         <is>
           <t>1</t>
@@ -1696,28 +1886,32 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics-IE-List</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>typeOfError</t>
+          <t>e2nodeComponentInterfaceTypeNG</t>
         </is>
       </c>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>TypeOfError</t>
+          <t>E2nodeComponentInterfaceNG</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1744,28 +1938,32 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>RICqueryFailure</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Container</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>RICqueryFailure</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>protocolIEs</t>
+          <t>e2nodeComponentInterfaceTypeXn</t>
         </is>
       </c>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
+          <t>E2nodeComponentInterfaceXn</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1782,65 +1980,45 @@
       <c r="N18" t="n">
         <v>-1</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>RICqueryFailure</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>unsuccessfulOutcome</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>id-RICquery</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>ricQuery</t>
-        </is>
-      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>id-RICrequestID</t>
+          <t>e2nodeComponentInterfaceTypeE1</t>
         </is>
       </c>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
+          <t>E2nodeComponentInterfaceE1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
@@ -1850,11 +2028,7 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>child_of_msg</t>
-        </is>
-      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
         <v>-1</v>
       </c>
@@ -1863,44 +2037,40 @@
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>RICqueryFailure</t>
-        </is>
-      </c>
+      <c r="T19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>id-RANfunctionID</t>
+          <t>e2nodeComponentInterfaceTypeF1</t>
         </is>
       </c>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>RANfunctionID</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>reject</t>
-        </is>
-      </c>
+          <t>E2nodeComponentInterfaceF1</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
@@ -1910,57 +2080,49 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>child_of_msg</t>
-        </is>
-      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>RICqueryFailure</t>
-        </is>
-      </c>
+      <c r="T20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>id-Cause</t>
+          <t>e2nodeComponentInterfaceTypeW1</t>
         </is>
       </c>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>Cause</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>ignore</t>
-        </is>
-      </c>
+          <t>E2nodeComponentInterfaceW1</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
@@ -1970,11 +2132,7 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>child_of_msg</t>
-        </is>
-      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
         <v>-1</v>
       </c>
@@ -1983,49 +2141,41 @@
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>RICqueryFailure</t>
-        </is>
-      </c>
+      <c r="T21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>RICqueryFailure-IEs</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>id-CriticalityDiagnostics</t>
+          <t>e2nodeComponentInterfaceTypeS1</t>
         </is>
       </c>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>CriticalityDiagnostics</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>ignore</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>OPTIONAL</t>
-        </is>
-      </c>
+          <t>E2nodeComponentInterfaceS1</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
           <t>1</t>
@@ -2034,11 +2184,7 @@
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>child_of_msg</t>
-        </is>
-      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
         <v>-1</v>
       </c>
@@ -2047,37 +2193,37 @@
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>RICqueryFailure</t>
-        </is>
-      </c>
+      <c r="T22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
+          <t>E2nodeComponentID</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SEQUENCE</t>
+          <t>CHOICE</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
+          <t>E2nodeComponentID</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>ricRequestorID</t>
+          <t>e2nodeComponentInterfaceTypeX2</t>
         </is>
       </c>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>INTEGER (0..65535)</t>
+          <t>E2nodeComponentInterfaceX2</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -2104,7 +2250,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
+          <t>E2nodeComponentInterfaceE1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2114,18 +2260,18 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>RICrequestID</t>
+          <t>E2nodeComponentInterfaceE1</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>ricInstanceID</t>
+          <t>gNB-CU-UP-ID</t>
         </is>
       </c>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>INTEGER (0..65535)</t>
+          <t>GNB-CU-UP-ID</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -2140,7 +2286,7 @@
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
@@ -2149,6 +2295,2178 @@
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceF1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceF1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>gNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>GNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="n">
+        <v>6</v>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceNG</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceNG</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>amf-name</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>AMFName</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="n">
+        <v>10</v>
+      </c>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceS1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceS1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>mme-name</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>MMEname</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="n">
+        <v>10</v>
+      </c>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceW1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceW1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>ng-eNB-DU-ID</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>NGENB-DU-ID</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="n">
+        <v>6</v>
+      </c>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>global-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceX2</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" s="1" t="inlineStr">
+        <is>
+          <t>global-en-gNB-ID</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceXn</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>E2nodeComponentInterfaceXn</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>global-NG-RAN-Node-ID</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>E2setupResponse</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Container</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>E2setupResponse</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" s="1" t="inlineStr">
+        <is>
+          <t>protocolIEs</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>E2setupResponse</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>successfulOutcome</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>id-E2setup</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>e2setup</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" s="1" t="inlineStr">
+        <is>
+          <t>id-TransactionID</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="inlineStr">
+        <is>
+          <t>TransactionID</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>child_of_msg</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>5</v>
+      </c>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>E2setupResponse</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>id-GlobalRIC-ID</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>GlobalRIC-ID</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>child_of_msg</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>E2setupResponse</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>id-RANfunctionsAccepted</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionsID-List</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>child_of_msg</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>E2setupResponse</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" s="1" t="inlineStr">
+        <is>
+          <t>id-RANfunctionsRejected</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionsIDcause-List</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>OPTIONAL</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>child_of_msg</t>
+        </is>
+      </c>
+      <c r="N36" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>E2setupResponse</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>E2setupResponseIEs</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" s="1" t="inlineStr">
+        <is>
+          <t>id-E2nodeComponentConfigAdditionAck</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="inlineStr">
+        <is>
+          <t>E2nodeComponentConfigAdditionAck-List</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>reject</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>child_of_msg</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>E2setupResponse</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E38" s="1" t="inlineStr">
+        <is>
+          <t>macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (20))</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E39" s="1" t="inlineStr">
+        <is>
+          <t>home-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (28))</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E40" s="1" t="inlineStr">
+        <is>
+          <t>short-Macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(18))</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>long-Macro-eNB-ID</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(21))</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E42" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-macro</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(20))</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E43" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-shortmacro</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(18))</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E44" s="1" t="inlineStr">
+        <is>
+          <t>enb-ID-longmacro</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(21))</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>gNB-ID</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (22..32))</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>gnb-ID</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE(22..32))</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" s="1" t="inlineStr">
+        <is>
+          <t>pLMN-Identity</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="n">
+        <v>8</v>
+      </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>GlobalENB-ID</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" s="1" t="inlineStr">
+        <is>
+          <t>eNB-ID</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="inlineStr">
+        <is>
+          <t>ENB-ID</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E49" s="1" t="inlineStr">
+        <is>
+          <t>gNB</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>CHOICE</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>GlobalNG-RANNode-ID</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E50" s="1" t="inlineStr">
+        <is>
+          <t>ng-eNB</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>GlobalRIC-ID</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>GlobalRIC-ID</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" s="1" t="inlineStr">
+        <is>
+          <t>pLMN-Identity</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="n">
+        <v>8</v>
+      </c>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>GlobalRIC-ID</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>GlobalRIC-ID</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" s="1" t="inlineStr">
+        <is>
+          <t>ric-ID</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="inlineStr">
+        <is>
+          <t>BIT STRING (SIZE (20))</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" s="1" t="inlineStr">
+        <is>
+          <t>pLMN-Identity</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="n">
+        <v>8</v>
+      </c>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>GlobalenGNB-ID</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" s="1" t="inlineStr">
+        <is>
+          <t>gNB-ID</t>
+        </is>
+      </c>
+      <c r="F54" s="1" t="inlineStr">
+        <is>
+          <t>ENGNB-ID</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" s="1" t="inlineStr">
+        <is>
+          <t>plmn-id</t>
+        </is>
+      </c>
+      <c r="F55" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="n">
+        <v>8</v>
+      </c>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>GlobalgNB-ID</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" s="1" t="inlineStr">
+        <is>
+          <t>gnb-id</t>
+        </is>
+      </c>
+      <c r="F56" s="1" t="inlineStr">
+        <is>
+          <t>GNB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" s="1" t="inlineStr">
+        <is>
+          <t>plmn-id</t>
+        </is>
+      </c>
+      <c r="F57" s="1" t="inlineStr">
+        <is>
+          <t>PLMN-Identity</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="n">
+        <v>8</v>
+      </c>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>GlobalngeNB-ID</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>enb-id</t>
+        </is>
+      </c>
+      <c r="F58" s="1" t="inlineStr">
+        <is>
+          <t>ENB-ID-Choice</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>RANfunctionID-Item</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>RANfunctionID-Item</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" s="1" t="inlineStr">
+        <is>
+          <t>ranFunctionID</t>
+        </is>
+      </c>
+      <c r="F59" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionID</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="n">
+        <v>6</v>
+      </c>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr"/>
+      <c r="T59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>RANfunctionID-Item</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>RANfunctionID-Item</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>ranFunctionRevision</t>
+        </is>
+      </c>
+      <c r="F60" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionRevision</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="n">
+        <v>6</v>
+      </c>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr"/>
+      <c r="T60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>RANfunctionID-ItemIEs</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>RANfunctionID-ItemIEs</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" s="1" t="inlineStr">
+        <is>
+          <t>id-RANfunctionID-Item</t>
+        </is>
+      </c>
+      <c r="F61" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionID-Item</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>ignore</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
+      <c r="S61" t="inlineStr"/>
+      <c r="T61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>RANfunctionIDcause-Item</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>RANfunctionIDcause-Item</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" s="1" t="inlineStr">
+        <is>
+          <t>ranFunctionID</t>
+        </is>
+      </c>
+      <c r="F62" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionID</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="n">
+        <v>6</v>
+      </c>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="inlineStr"/>
+      <c r="T62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>RANfunctionIDcause-Item</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SEQUENCE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>RANfunctionIDcause-Item</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" s="1" t="inlineStr">
+        <is>
+          <t>cause</t>
+        </is>
+      </c>
+      <c r="F63" s="1" t="inlineStr">
+        <is>
+          <t>Cause</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
+      <c r="S63" t="inlineStr"/>
+      <c r="T63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>RANfunctionIDcause-ItemIEs</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>RANfunctionIDcause-ItemIEs</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" s="1" t="inlineStr">
+        <is>
+          <t>id-RANfunctionIEcause-Item</t>
+        </is>
+      </c>
+      <c r="F64" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionIDcause-Item</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>ignore</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="inlineStr"/>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>RANfunctionsID-List</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SingleContainer</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionsID-List</t>
+        </is>
+      </c>
+      <c r="F65" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionID-ItemIEs</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>256</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
+      <c r="R65" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
+      <c r="T65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>RANfunctionsIDcause-List</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SingleContainer</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionsIDcause-List</t>
+        </is>
+      </c>
+      <c r="F66" s="1" t="inlineStr">
+        <is>
+          <t>RANfunctionIDcause-ItemIEs</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>256</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
+      <c r="R66" t="inlineStr"/>
+      <c r="S66" t="inlineStr"/>
+      <c r="T66" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>